<commit_message>
Updates the schedules to reflect new curriculum
</commit_message>
<xml_diff>
--- a/course-info/OCP21 Info Schedules and variants.xlsx
+++ b/course-info/OCP21 Info Schedules and variants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kramor/Development/Projects/Yoink/ocp-21/course-info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A72932-163C-DF40-AD2A-5032A4FEE742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0F74BD-2AD4-F443-AF5C-A4E6477EE6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{1E2FBF5C-1E84-9C41-A233-7939A783596D}"/>
+    <workbookView xWindow="30340" yWindow="-7040" windowWidth="29920" windowHeight="33140" activeTab="1" xr2:uid="{1E2FBF5C-1E84-9C41-A233-7939A783596D}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
   <si>
     <t>Week</t>
   </si>
@@ -93,21 +93,9 @@
     <t>10-Week variant</t>
   </si>
   <si>
-    <t>20-Week variant</t>
-  </si>
-  <si>
     <t>Review CH1-4</t>
   </si>
   <si>
-    <t>CH1</t>
-  </si>
-  <si>
-    <t>CH2 &amp; CH3</t>
-  </si>
-  <si>
-    <t>CH4</t>
-  </si>
-  <si>
     <t>CH1 &amp; CH2</t>
   </si>
   <si>
@@ -135,9 +123,6 @@
     <t>CH13</t>
   </si>
   <si>
-    <t>CH14 &amp; CH15</t>
-  </si>
-  <si>
     <t>CH7</t>
   </si>
   <si>
@@ -150,51 +135,15 @@
     <t>Review CH9-10</t>
   </si>
   <si>
-    <t>CH11</t>
-  </si>
-  <si>
-    <t>CH12</t>
-  </si>
-  <si>
-    <t>Review CH11-13</t>
-  </si>
-  <si>
     <t>CH14</t>
   </si>
   <si>
-    <t>CH15</t>
-  </si>
-  <si>
-    <t>Review CH14-15</t>
-  </si>
-  <si>
-    <t>Review CH1-15</t>
-  </si>
-  <si>
-    <t>Database access, JDBC</t>
-  </si>
-  <si>
-    <t>Modules</t>
-  </si>
-  <si>
-    <t>Exceptions, Localization, Resource Management</t>
-  </si>
-  <si>
     <t>Lambdas</t>
   </si>
   <si>
     <t>Interfaces, Enums, Records, Nesting</t>
   </si>
   <si>
-    <t>Java Core APIs (String, Date, Math)</t>
-  </si>
-  <si>
-    <t>Working with variables &amp; values and control flow</t>
-  </si>
-  <si>
-    <t>Basics of Java and JVM</t>
-  </si>
-  <si>
     <t>Course Information Card</t>
   </si>
   <si>
@@ -376,6 +325,21 @@
   </si>
   <si>
     <t>The most notable addition of material is the inclusion of Virtual Threads, which can be found in the Chapter 13 - Concurrency.</t>
+  </si>
+  <si>
+    <t>15-Week variant</t>
+  </si>
+  <si>
+    <t>I/O, Files</t>
+  </si>
+  <si>
+    <t>Basics of Java and JVM, Working with variables</t>
+  </si>
+  <si>
+    <t>Exceptions, Localization, Resource Management, Modules</t>
+  </si>
+  <si>
+    <t>Review CH1-14</t>
   </si>
 </sst>
 </file>
@@ -773,7 +737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8B40A1-F1B2-8249-B314-FEC84FEA588F}">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -784,306 +748,306 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1093,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1126F6-B530-B244-81F4-BD52E58F1A60}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1134,7 +1098,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -1148,7 +1112,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1159,7 +1123,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -1170,7 +1134,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -1181,7 +1145,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1192,7 +1156,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1203,7 +1167,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -1214,7 +1178,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -1225,7 +1189,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -1242,12 +1206,12 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1269,10 +1233,10 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -1283,10 +1247,10 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1294,10 +1258,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1305,10 +1266,10 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1316,10 +1277,10 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1327,10 +1288,10 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1338,10 +1299,10 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
         <v>33</v>
-      </c>
-      <c r="C25" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1349,10 +1310,7 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1360,7 +1318,10 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1368,10 +1329,10 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1379,10 +1340,7 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1390,7 +1348,10 @@
         <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1398,10 +1359,13 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1409,70 +1373,18 @@
         <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>16</v>
-      </c>
-      <c r="B34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>17</v>
-      </c>
-      <c r="B35" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>18</v>
-      </c>
-      <c r="B36" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>19</v>
-      </c>
-      <c r="B37" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>20</v>
-      </c>
-      <c r="B38" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New additions from OCP Kadaster Course
</commit_message>
<xml_diff>
--- a/course-info/OCP21 Info Schedules and variants.xlsx
+++ b/course-info/OCP21 Info Schedules and variants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kramor/Development/Projects/Yoink/ocp-21/course-info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0F74BD-2AD4-F443-AF5C-A4E6477EE6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F3DB5B-BE81-5A41-9833-2EFFC33B3E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30340" yWindow="-7040" windowWidth="29920" windowHeight="33140" activeTab="1" xr2:uid="{1E2FBF5C-1E84-9C41-A233-7939A783596D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29920" windowHeight="18880" activeTab="1" xr2:uid="{1E2FBF5C-1E84-9C41-A233-7939A783596D}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="118">
   <si>
     <t>Week</t>
   </si>
@@ -340,6 +340,57 @@
   </si>
   <si>
     <t>Review CH1-14</t>
+  </si>
+  <si>
+    <t>20-Week variant</t>
+  </si>
+  <si>
+    <t>CH1</t>
+  </si>
+  <si>
+    <t>Basics of Java and JVM</t>
+  </si>
+  <si>
+    <t>CH2 &amp; CH3</t>
+  </si>
+  <si>
+    <t>Working with variables &amp; values and control flow</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>Java Core APIs (String, Date, Math)</t>
+  </si>
+  <si>
+    <t>CH11</t>
+  </si>
+  <si>
+    <t>Exceptions, Localization, Resource Management</t>
+  </si>
+  <si>
+    <t>CH12</t>
+  </si>
+  <si>
+    <t>Modules</t>
+  </si>
+  <si>
+    <t>Review CH1-15</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Kick-off / Planning</t>
+  </si>
+  <si>
+    <t>Check if everyone has received a book and Enthuware licenses. If necessary, assist with installing Enthuware. Make planning. Shorter session (&lt;2hr)</t>
+  </si>
+  <si>
+    <t>Review CH11-12</t>
+  </si>
+  <si>
+    <t>Review CH13-14</t>
   </si>
 </sst>
 </file>
@@ -1057,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1126F6-B530-B244-81F4-BD52E58F1A60}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A36" sqref="A36:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,12 +1430,242 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>15</v>
       </c>
       <c r="B33" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>11</v>
+      </c>
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>12</v>
+      </c>
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>13</v>
+      </c>
+      <c r="B50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>15</v>
+      </c>
+      <c r="B52" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>16</v>
+      </c>
+      <c r="B53" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>17</v>
+      </c>
+      <c r="B54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>18</v>
+      </c>
+      <c r="B55" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>19</v>
+      </c>
+      <c r="B56" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>20</v>
+      </c>
+      <c r="B57" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>